<commit_message>
added DEBUG_PRINT and set test servo angles to ~90 degrees
</commit_message>
<xml_diff>
--- a/kinematics/delta kinematics test.xlsx
+++ b/kinematics/delta kinematics test.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="20100" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="14100" windowHeight="16080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Base</t>
   </si>
@@ -64,9 +69,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t>servoAngle</t>
-  </si>
-  <si>
     <t>WARNING: arguments to Excel's ATAN2 function are reversed from normal convention!</t>
   </si>
   <si>
@@ -80,13 +82,22 @@
   </si>
   <si>
     <t>Results:</t>
+  </si>
+  <si>
+    <t>gripper</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>ServoAngle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +110,22 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -125,11 +152,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -138,7 +165,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -146,17 +173,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -166,7 +193,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -174,12 +201,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -188,26 +215,28 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -223,8 +252,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,37 +560,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8">
       <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -563,19 +599,19 @@
         <v>7</v>
       </c>
       <c r="G5" s="13">
-        <f>C5*COS(RADIANS(C15))-C7*SIN(RADIANS(C15))</f>
-        <v>0.44828773608402683</v>
+        <f>C5*COS(RADIANS(C16))-C7*SIN(RADIANS(C16))</f>
+        <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5">
-        <v>-10</v>
+        <v>-61.284999999999997</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>15</v>
@@ -584,19 +620,19 @@
         <v>8</v>
       </c>
       <c r="G6" s="12">
-        <f>C6</f>
-        <v>-10</v>
+        <f>C6+C15</f>
+        <v>-44.284999999999997</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>15</v>
@@ -605,58 +641,58 @@
         <v>9</v>
       </c>
       <c r="G7" s="12">
-        <f>C5*SIN(RADIANS(C15))+C7*COS(RADIANS(C15))</f>
-        <v>2.1906706976806571</v>
+        <f>C5*SIN(RADIANS(C16))+C7*COS(RADIANS(C16))</f>
+        <v>0</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8">
       <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="12">
         <f>SQRT((G5+C12-C11)^2+G6^2)</f>
-        <v>10.119674448814409</v>
+        <v>44.310396353451857</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8">
       <c r="F9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="12">
         <f>SQRT(C14^2-G7^2)</f>
-        <v>9.7570980262741713</v>
+        <v>51.1</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="12">
         <f>DEGREES(ACOS((-(G9^2)+C13^2+G8^2)/(2*C13*G8)))</f>
-        <v>63.910169780708522</v>
+        <v>91.934529309567537</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>15</v>
@@ -666,68 +702,94 @@
       </c>
       <c r="G11" s="12">
         <f>DEGREES(ATAN2(G5+C12-C11,G6))</f>
-        <v>-98.820313118531246</v>
+        <v>-91.939953138537973</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8">
       <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="14">
+      <c r="F12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="19">
         <f>G10-ABS(G11)</f>
-        <v>-34.910143337822724</v>
-      </c>
-      <c r="H12" s="9" t="s">
+        <v>-5.4238289704358067E-3</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8">
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="5">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="14">
+        <f>G12+90</f>
+        <v>89.994576171029564</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
       <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="5">
-        <v>10</v>
+        <v>51.1</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="8">
-        <v>15</v>
-      </c>
-      <c r="D15" s="9" t="s">
+    <row r="15" spans="2:8">
+      <c r="B15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="16">
+        <v>17</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>